<commit_message>
rewriting code for species slopes
</commit_message>
<xml_diff>
--- a/results/species-results.xlsx
+++ b/results/species-results.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/My Drive/My_Drive_Cloud/Drive-Projects/Pepperwood/Pepperwood_git_projects/PepperwoodLFM/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/github/pepperwood/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{85176E88-F24A-BD4E-8212-D669B0649558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BD8974-F2FA-0D47-997C-89C92555415C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="760" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="580" yWindow="760" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species-results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -202,9 +215,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -691,7 +704,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1048,11 +1061,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>